<commit_message>
Add Listed subscriptions Report
</commit_message>
<xml_diff>
--- a/reports/listed_products_report/templates/xlsx/template.xlsx
+++ b/reports/listed_products_report/templates/xlsx/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\global-connect-reports\reports\listed_products_report\templates\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E5EBBCF-4725-465D-81BB-2AA96505DBFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05F5C6C-3AE0-43AB-B22E-EC490A27645E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$Q$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Exported At</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Business Contact</t>
+  </si>
+  <si>
+    <t>Last Version Date</t>
   </si>
 </sst>
 </file>
@@ -432,24 +435,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="25.81640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="10" width="21.6328125" customWidth="1"/>
-    <col min="11" max="11" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="13" width="45.81640625" customWidth="1"/>
-    <col min="14" max="14" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="16" width="21.1796875" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="15.08984375" customWidth="1"/>
+    <col min="5" max="11" width="21.6328125" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="14" width="45.81640625" customWidth="1"/>
+    <col min="15" max="15" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="17" width="21.1796875" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -475,35 +478,38 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:R1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>